<commit_message>
measure data of Tr TEGs
added measure data of Tr TEGs
</commit_message>
<xml_diff>
--- a/151009measureR.xlsx
+++ b/151009measureR.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akita\Documents\Dropbox\1Project\MkLSI\github\makelsi\Measure\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="12915" windowHeight="10320" activeTab="3"/>
   </bookViews>
@@ -12,7 +17,7 @@
     <sheet name="24-25" sheetId="3" r:id="rId3"/>
     <sheet name="21-25" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -327,6 +332,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -674,11 +682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94749248"/>
-        <c:axId val="94749824"/>
+        <c:axId val="189679824"/>
+        <c:axId val="189680384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94749248"/>
+        <c:axId val="189679824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,12 +696,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94749824"/>
+        <c:crossAx val="189680384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94749824"/>
+        <c:axId val="189680384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,7 +712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94749248"/>
+        <c:crossAx val="189679824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -830,11 +838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92907776"/>
-        <c:axId val="92907200"/>
+        <c:axId val="189683184"/>
+        <c:axId val="189683744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92907776"/>
+        <c:axId val="189683184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,12 +852,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92907200"/>
+        <c:crossAx val="189683744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92907200"/>
+        <c:axId val="189683744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -860,7 +868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92907776"/>
+        <c:crossAx val="189683184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -998,11 +1006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120936064"/>
-        <c:axId val="120935488"/>
+        <c:axId val="189685984"/>
+        <c:axId val="189686544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120936064"/>
+        <c:axId val="189685984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,12 +1020,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120935488"/>
+        <c:crossAx val="189686544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120935488"/>
+        <c:axId val="189686544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120936064"/>
+        <c:crossAx val="189685984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1160,11 +1168,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93581248"/>
-        <c:axId val="93580672"/>
+        <c:axId val="192113248"/>
+        <c:axId val="192113808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93581248"/>
+        <c:axId val="192113248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,12 +1182,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93580672"/>
+        <c:crossAx val="192113808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93580672"/>
+        <c:axId val="192113808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93581248"/>
+        <c:crossAx val="192113248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,7 +1361,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1395,7 +1403,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1430,7 +1438,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2139,7 +2147,8 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>